<commit_message>
Ran baseline model on whole data and scored it.
</commit_message>
<xml_diff>
--- a/simplyJapanese/data/2_ProcessedData/Combined_85K_150.xlsx_baseline_predictions.xlsx
+++ b/simplyJapanese/data/2_ProcessedData/Combined_85K_150.xlsx_baseline_predictions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="37320" windowHeight="18315"/>
+    <workbookView xWindow="2160" yWindow="0" windowWidth="37320" windowHeight="18315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1635,11 +1635,12 @@
   <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>

</xml_diff>